<commit_message>
Removed unused alpha diversity metrics
</commit_message>
<xml_diff>
--- a/Content_Mucosa_Comparison.xlsx
+++ b/Content_Mucosa_Comparison.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/7ecf4928fe261446/Documents/GitHub/Cecum_Microbes/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{8685928E-8C3E-4FC9-AD9F-C09EC18B1399}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="13" documentId="8_{8685928E-8C3E-4FC9-AD9F-C09EC18B1399}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{1084FE2B-AEE5-4E5C-B166-4AC955361453}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{B128C7AB-569C-4147-8A87-E56A796A8D1E}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{B128C7AB-569C-4147-8A87-E56A796A8D1E}"/>
   </bookViews>
   <sheets>
     <sheet name="Content-Mucosa Comparison" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="244" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="149" uniqueCount="29">
   <si>
     <t>Group</t>
   </si>
@@ -67,21 +67,12 @@
     <t>Metric</t>
   </si>
   <si>
-    <t>Total OTUs</t>
-  </si>
-  <si>
-    <t>Bergerparker</t>
-  </si>
-  <si>
     <t>Chao</t>
   </si>
   <si>
     <t>Shannon</t>
   </si>
   <si>
-    <t>Inverse Simpson</t>
-  </si>
-  <si>
     <t>Bray-Curtis PERMANOVA</t>
   </si>
   <si>
@@ -122,9 +113,6 @@
   </si>
   <si>
     <t>Torpor vs. Spring</t>
-  </si>
-  <si>
-    <t>Summer_wild vs. Spring</t>
   </si>
   <si>
     <t>Summer_wild vs. IBA</t>
@@ -177,7 +165,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="4">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -200,17 +188,6 @@
       <top style="thin">
         <color indexed="64"/>
       </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
       <bottom/>
       <diagonal/>
     </border>
@@ -218,22 +195,19 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
@@ -552,10 +526,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2DC80A74-2A10-4D54-885F-E55396169400}">
-  <dimension ref="A1:I26"/>
+  <dimension ref="A1:I11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E24" sqref="E24"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H19" sqref="H19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -605,7 +579,7 @@
         <v>10</v>
       </c>
       <c r="D2">
-        <v>0.46939999999999998</v>
+        <v>0.38240000000000002</v>
       </c>
       <c r="F2" t="s">
         <v>3</v>
@@ -614,7 +588,7 @@
         <v>4</v>
       </c>
       <c r="H2" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="I2">
         <v>0.7</v>
@@ -631,7 +605,7 @@
         <v>10</v>
       </c>
       <c r="D3">
-        <v>0.7782</v>
+        <v>0.82650000000000001</v>
       </c>
       <c r="F3" t="s">
         <v>5</v>
@@ -640,7 +614,7 @@
         <v>4</v>
       </c>
       <c r="H3" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="I3">
         <v>0.97299999999999998</v>
@@ -657,7 +631,7 @@
         <v>10</v>
       </c>
       <c r="D4">
-        <v>0.7268</v>
+        <v>3.3309999999999999E-2</v>
       </c>
       <c r="F4" t="s">
         <v>6</v>
@@ -666,7 +640,7 @@
         <v>4</v>
       </c>
       <c r="H4" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="I4">
         <v>0.94099999999999995</v>
@@ -683,7 +657,7 @@
         <v>10</v>
       </c>
       <c r="D5">
-        <v>0.45429999999999998</v>
+        <v>0.43180000000000002</v>
       </c>
       <c r="F5" t="s">
         <v>7</v>
@@ -692,7 +666,7 @@
         <v>4</v>
       </c>
       <c r="H5" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="I5">
         <v>0.95099999999999996</v>
@@ -709,7 +683,7 @@
         <v>10</v>
       </c>
       <c r="D6" s="3">
-        <v>0.38300000000000001</v>
+        <v>0.92520000000000002</v>
       </c>
       <c r="F6" s="4" t="s">
         <v>8</v>
@@ -718,7 +692,7 @@
         <v>4</v>
       </c>
       <c r="H6" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="I6" s="4">
         <v>0.9</v>
@@ -735,7 +709,7 @@
         <v>11</v>
       </c>
       <c r="D7">
-        <v>0.4</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.3">
@@ -749,7 +723,7 @@
         <v>11</v>
       </c>
       <c r="D8">
-        <v>0.28920000000000001</v>
+        <v>0.3654</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.3">
@@ -763,7 +737,7 @@
         <v>11</v>
       </c>
       <c r="D9">
-        <v>0.70820000000000005</v>
+        <v>0.4803</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.3">
@@ -777,7 +751,7 @@
         <v>11</v>
       </c>
       <c r="D10">
-        <v>1</v>
+        <v>0.47589999999999999</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.3">
@@ -791,217 +765,7 @@
         <v>11</v>
       </c>
       <c r="D11" s="3">
-        <v>0.19969999999999999</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A12" t="s">
-        <v>3</v>
-      </c>
-      <c r="B12" t="s">
-        <v>4</v>
-      </c>
-      <c r="C12" t="s">
-        <v>12</v>
-      </c>
-      <c r="D12">
-        <v>0.38240000000000002</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A13" t="s">
-        <v>5</v>
-      </c>
-      <c r="B13" t="s">
-        <v>4</v>
-      </c>
-      <c r="C13" t="s">
-        <v>12</v>
-      </c>
-      <c r="D13">
-        <v>0.82650000000000001</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A14" t="s">
-        <v>6</v>
-      </c>
-      <c r="B14" t="s">
-        <v>4</v>
-      </c>
-      <c r="C14" t="s">
-        <v>12</v>
-      </c>
-      <c r="D14">
-        <v>3.3309999999999999E-2</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A15" t="s">
-        <v>7</v>
-      </c>
-      <c r="B15" t="s">
-        <v>4</v>
-      </c>
-      <c r="C15" t="s">
-        <v>12</v>
-      </c>
-      <c r="D15">
-        <v>0.43180000000000002</v>
-      </c>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A16" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="B16" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="C16" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="D16" s="3">
-        <v>0.92520000000000002</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A17" t="s">
-        <v>3</v>
-      </c>
-      <c r="B17" t="s">
-        <v>4</v>
-      </c>
-      <c r="C17" t="s">
-        <v>13</v>
-      </c>
-      <c r="D17">
-        <v>0.2</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A18" t="s">
-        <v>5</v>
-      </c>
-      <c r="B18" t="s">
-        <v>4</v>
-      </c>
-      <c r="C18" t="s">
-        <v>13</v>
-      </c>
-      <c r="D18">
-        <v>0.3654</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A19" t="s">
-        <v>6</v>
-      </c>
-      <c r="B19" t="s">
-        <v>4</v>
-      </c>
-      <c r="C19" t="s">
-        <v>13</v>
-      </c>
-      <c r="D19">
-        <v>0.4803</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A20" t="s">
-        <v>7</v>
-      </c>
-      <c r="B20" t="s">
-        <v>4</v>
-      </c>
-      <c r="C20" t="s">
-        <v>13</v>
-      </c>
-      <c r="D20">
-        <v>0.47589999999999999</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A21" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="B21" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="C21" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="D21" s="3">
         <v>0.11119999999999999</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A22" t="s">
-        <v>3</v>
-      </c>
-      <c r="B22" t="s">
-        <v>4</v>
-      </c>
-      <c r="C22" t="s">
-        <v>14</v>
-      </c>
-      <c r="D22">
-        <v>0.13</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A23" t="s">
-        <v>5</v>
-      </c>
-      <c r="B23" t="s">
-        <v>4</v>
-      </c>
-      <c r="C23" t="s">
-        <v>14</v>
-      </c>
-      <c r="D23">
-        <v>0.68810000000000004</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A24" t="s">
-        <v>6</v>
-      </c>
-      <c r="B24" t="s">
-        <v>4</v>
-      </c>
-      <c r="C24" t="s">
-        <v>14</v>
-      </c>
-      <c r="D24">
-        <v>0.57689999999999997</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A25" t="s">
-        <v>7</v>
-      </c>
-      <c r="B25" t="s">
-        <v>4</v>
-      </c>
-      <c r="C25" t="s">
-        <v>14</v>
-      </c>
-      <c r="D25">
-        <v>0.63890000000000002</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A26" s="11" t="s">
-        <v>8</v>
-      </c>
-      <c r="B26" s="11" t="s">
-        <v>4</v>
-      </c>
-      <c r="C26" s="11" t="s">
-        <v>14</v>
-      </c>
-      <c r="D26" s="11">
-        <v>2.7369999999999998E-2</v>
       </c>
     </row>
   </sheetData>
@@ -1012,10 +776,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5A86CB5D-939B-4B14-AC59-EE530224E751}">
-  <dimension ref="A1:K34"/>
+  <dimension ref="A1:K31"/>
   <sheetViews>
-    <sheetView topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="F22" sqref="F22"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D24" sqref="D24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1056,144 +820,136 @@
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A2" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="B2" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="C2" s="7" t="s">
+      <c r="A2" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="B2" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="C2" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="D2" s="7">
-        <v>1.6469999999999999E-2</v>
+      <c r="D2" s="9">
+        <v>2.6440000000000002E-2</v>
       </c>
       <c r="G2" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="H2" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="I2" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="J2">
         <v>1E-3</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A3" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="B3" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="C3" s="4" t="s">
+      <c r="A3" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="B3" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="C3" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="D3" s="4">
-        <v>1.1469999999999999E-2</v>
+      <c r="D3" s="10">
+        <v>0.1638</v>
       </c>
       <c r="G3" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="H3" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="I3" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="J3">
         <v>1E-3</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A4" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="B4" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="C4" s="3" t="s">
+      <c r="A4" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="B4" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="C4" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="D4" s="3">
-        <v>2.23E-5</v>
+      <c r="D4" s="8">
+        <v>1.2619999999999999E-2</v>
       </c>
       <c r="G4" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="H4" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="I4" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="J4">
         <v>1E-3</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A5" s="10" t="s">
+      <c r="A5" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="B5" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="C5" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="D5" s="9">
+        <v>1.9499999999999999E-3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A6" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="B6" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="C6" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="D6" s="10">
+        <v>0.751</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A7" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="B5" s="10" t="s">
-        <v>18</v>
-      </c>
-      <c r="C5" s="10" t="s">
+      <c r="B7" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="C7" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="D5" s="10">
-        <v>5.8709999999999998E-2</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A6" s="5" t="s">
+      <c r="D7" s="8">
+        <v>9.0299999999999998E-3</v>
+      </c>
+      <c r="G7" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="B6" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="C6" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="D6" s="5">
-        <v>0.91659999999999997</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A7" s="9" t="s">
-        <v>19</v>
-      </c>
-      <c r="B7" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="C7" s="9" t="s">
-        <v>11</v>
-      </c>
-      <c r="D7" s="9">
-        <v>0.1588</v>
-      </c>
-      <c r="G7" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="H7" s="6"/>
-      <c r="I7" s="6"/>
-      <c r="J7" s="6"/>
+      <c r="H7" s="5"/>
+      <c r="I7" s="5"/>
+      <c r="J7" s="5"/>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A8" s="12" t="s">
-        <v>16</v>
-      </c>
-      <c r="B8" s="12" t="s">
-        <v>18</v>
-      </c>
-      <c r="C8" s="12" t="s">
-        <v>12</v>
-      </c>
-      <c r="D8" s="12">
-        <v>2.6440000000000002E-2</v>
-      </c>
+      <c r="A8" s="7"/>
+      <c r="B8" s="7"/>
+      <c r="C8" s="7"/>
+      <c r="D8" s="7"/>
       <c r="G8" s="2" t="s">
         <v>0</v>
       </c>
@@ -1204,447 +960,263 @@
         <v>9</v>
       </c>
       <c r="J8" s="2" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A9" s="13" t="s">
+      <c r="G9" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="H9" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="I9" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="J9" s="11" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A10" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="B9" s="13" t="s">
-        <v>18</v>
-      </c>
-      <c r="C9" s="13" t="s">
-        <v>12</v>
-      </c>
-      <c r="D9" s="13">
-        <v>0.1638</v>
-      </c>
-      <c r="G9" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="H9" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="I9" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="J9" s="14" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A10" s="11" t="s">
-        <v>19</v>
-      </c>
-      <c r="B10" s="11" t="s">
-        <v>18</v>
-      </c>
-      <c r="C10" s="11" t="s">
-        <v>12</v>
-      </c>
-      <c r="D10" s="11">
-        <v>1.2619999999999999E-2</v>
-      </c>
+      <c r="B10" s="5"/>
+      <c r="C10" s="5"/>
+      <c r="D10" s="5"/>
       <c r="G10" s="4"/>
       <c r="H10" s="4"/>
       <c r="I10" s="4"/>
-      <c r="J10" s="16" t="s">
-        <v>23</v>
+      <c r="J10" s="13" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A11" s="12" t="s">
-        <v>16</v>
-      </c>
-      <c r="B11" s="12" t="s">
+      <c r="A11" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D11" s="2" t="s">
         <v>18</v>
-      </c>
-      <c r="C11" s="12" t="s">
-        <v>13</v>
-      </c>
-      <c r="D11" s="12">
-        <v>1.9499999999999999E-3</v>
       </c>
       <c r="G11" s="4"/>
       <c r="H11" s="4"/>
       <c r="I11" s="4"/>
-      <c r="J11" s="16" t="s">
+      <c r="J11" s="13" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A12" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="B12" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="C12" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="D12" s="6" t="s">
         <v>22</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A12" s="13" t="s">
-        <v>17</v>
-      </c>
-      <c r="B12" s="13" t="s">
-        <v>18</v>
-      </c>
-      <c r="C12" s="13" t="s">
-        <v>13</v>
-      </c>
-      <c r="D12" s="13">
-        <v>0.751</v>
       </c>
       <c r="G12" s="4"/>
       <c r="H12" s="4"/>
       <c r="I12" s="4"/>
-      <c r="J12" s="13" t="s">
-        <v>25</v>
+      <c r="J12" s="10" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A13" s="11" t="s">
-        <v>19</v>
-      </c>
-      <c r="B13" s="11" t="s">
-        <v>18</v>
-      </c>
-      <c r="C13" s="11" t="s">
-        <v>13</v>
-      </c>
-      <c r="D13" s="11">
-        <v>9.0299999999999998E-3</v>
+      <c r="A13" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D13" s="3" t="s">
+        <v>22</v>
       </c>
       <c r="G13" s="4"/>
       <c r="H13" s="4"/>
       <c r="I13" s="4"/>
-      <c r="J13" s="16" t="s">
-        <v>31</v>
+      <c r="J13" s="13" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A14" s="12" t="s">
-        <v>16</v>
-      </c>
-      <c r="B14" s="12" t="s">
-        <v>18</v>
-      </c>
-      <c r="C14" s="12" t="s">
-        <v>14</v>
-      </c>
-      <c r="D14" s="12">
-        <v>2.9749999999999999E-2</v>
+      <c r="A14" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="B14" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="C14" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="D14" s="6" t="s">
+        <v>23</v>
       </c>
       <c r="G14" s="4"/>
       <c r="H14" s="4"/>
       <c r="I14" s="4"/>
-      <c r="J14" s="16" t="s">
-        <v>24</v>
+      <c r="J14" s="13" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A15" s="13" t="s">
-        <v>17</v>
-      </c>
-      <c r="B15" s="13" t="s">
-        <v>18</v>
-      </c>
-      <c r="C15" s="13" t="s">
-        <v>14</v>
-      </c>
-      <c r="D15" s="13">
-        <v>0.96699999999999997</v>
+      <c r="A15" s="4"/>
+      <c r="B15" s="4"/>
+      <c r="C15" s="4"/>
+      <c r="D15" s="4" t="s">
+        <v>22</v>
       </c>
       <c r="G15" s="4"/>
       <c r="H15" s="4"/>
       <c r="I15" s="4"/>
-      <c r="J15" s="16" t="s">
-        <v>27</v>
+      <c r="J15" s="13" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A16" s="11" t="s">
-        <v>19</v>
-      </c>
-      <c r="B16" s="11" t="s">
-        <v>18</v>
-      </c>
-      <c r="C16" s="11" t="s">
-        <v>14</v>
-      </c>
-      <c r="D16" s="11">
-        <v>0.1124</v>
+      <c r="A16" s="4"/>
+      <c r="B16" s="4"/>
+      <c r="C16" s="4"/>
+      <c r="D16" s="4" t="s">
+        <v>25</v>
       </c>
       <c r="G16" s="3"/>
       <c r="H16" s="3"/>
       <c r="I16" s="3"/>
-      <c r="J16" s="18" t="s">
-        <v>28</v>
+      <c r="J16" s="15" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A17" s="4"/>
       <c r="B17" s="4"/>
       <c r="C17" s="4"/>
-      <c r="D17" s="4"/>
+      <c r="D17" s="4" t="s">
+        <v>24</v>
+      </c>
       <c r="G17" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="H17" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="I17" t="s">
-        <v>15</v>
-      </c>
-      <c r="J17" s="15" t="s">
-        <v>26</v>
+        <v>12</v>
+      </c>
+      <c r="J17" s="12" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A18" s="6" t="s">
+      <c r="A18" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B18" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C18" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D18" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="E18" s="1"/>
+      <c r="J18" s="12" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="J19" s="12" t="s">
         <v>20</v>
       </c>
-      <c r="B18" s="6"/>
-      <c r="C18" s="6"/>
-      <c r="D18" s="6"/>
-      <c r="E18" s="1"/>
-      <c r="J18" s="15" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A19" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B19" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C19" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="D19" s="2" t="s">
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="J20" s="12" t="s">
         <v>21</v>
       </c>
-      <c r="J19" s="15" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A20" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="B20" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="C20" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="D20" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="J20" s="15" t="s">
-        <v>24</v>
-      </c>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A21" s="4"/>
-      <c r="B21" s="4"/>
-      <c r="C21" s="4"/>
-      <c r="D21" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="J21" s="15" t="s">
-        <v>32</v>
+      <c r="J21" s="12" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A22" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="B22" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="C22" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="D22" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="J22" s="15" t="s">
-        <v>28</v>
+      <c r="J22" s="12" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A23" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="B23" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="C23" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="D23" s="4" t="s">
-        <v>22</v>
-      </c>
       <c r="G23" s="3"/>
       <c r="H23" s="3"/>
       <c r="I23" s="3"/>
-      <c r="J23" s="18" t="s">
-        <v>27</v>
+      <c r="J23" s="15" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A24" s="4"/>
-      <c r="B24" s="4"/>
-      <c r="C24" s="4"/>
-      <c r="D24" s="4" t="s">
+      <c r="G24" t="s">
+        <v>16</v>
+      </c>
+      <c r="H24" t="s">
+        <v>15</v>
+      </c>
+      <c r="I24" t="s">
+        <v>12</v>
+      </c>
+      <c r="J24" s="12" t="s">
         <v>23</v>
       </c>
-      <c r="G24" t="s">
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="J25" s="12" t="s">
         <v>19</v>
       </c>
-      <c r="H24" t="s">
-        <v>18</v>
-      </c>
-      <c r="I24" t="s">
-        <v>15</v>
-      </c>
-      <c r="J24" s="15" t="s">
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="J26" s="12" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A25" s="3"/>
-      <c r="B25" s="3"/>
-      <c r="C25" s="3"/>
-      <c r="D25" s="3" t="s">
+    <row r="27" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="J27" s="14" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="J28" s="12" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="29" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="J29" s="12" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="30" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="J30" s="12" t="s">
         <v>24</v>
       </c>
-      <c r="J25" s="15" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A26" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="B26" s="8" t="s">
-        <v>18</v>
-      </c>
-      <c r="C26" s="8" t="s">
-        <v>11</v>
-      </c>
-      <c r="D26" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="J26" s="15" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A27" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="B27" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="C27" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="D27" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="J27" s="17" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A28" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="B28" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="C28" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="D28" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="J28" s="15" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A29" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="B29" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="C29" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="D29" s="7" t="s">
-        <v>26</v>
-      </c>
-      <c r="J29" s="15" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A30" s="4"/>
-      <c r="B30" s="4"/>
-      <c r="C30" s="4"/>
-      <c r="D30" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="J30" s="15" t="s">
-        <v>27</v>
-      </c>
     </row>
     <row r="31" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A31" s="4"/>
-      <c r="B31" s="4"/>
-      <c r="C31" s="4"/>
-      <c r="D31" s="4" t="s">
-        <v>28</v>
-      </c>
       <c r="G31" s="3"/>
       <c r="H31" s="3"/>
       <c r="I31" s="3"/>
-      <c r="J31" s="18" t="s">
-        <v>28</v>
+      <c r="J31" s="15" t="s">
+        <v>25</v>
       </c>
       <c r="K31" s="3"/>
-    </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A32" s="4"/>
-      <c r="B32" s="4"/>
-      <c r="C32" s="4"/>
-      <c r="D32" s="4" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A33" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="B33" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="C33" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="D33" s="3" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A34" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="B34" s="8" t="s">
-        <v>18</v>
-      </c>
-      <c r="C34" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="D34" s="8" t="s">
-        <v>29</v>
-      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Cleaned up comparison stats; added lab comparisons and overall
</commit_message>
<xml_diff>
--- a/Content_Mucosa_Comparison.xlsx
+++ b/Content_Mucosa_Comparison.xlsx
@@ -8,13 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/7ecf4928fe261446/Documents/GitHub/Cecum_Microbes/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="13" documentId="8_{8685928E-8C3E-4FC9-AD9F-C09EC18B1399}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{1084FE2B-AEE5-4E5C-B166-4AC955361453}"/>
+  <xr:revisionPtr revIDLastSave="192" documentId="8_{8685928E-8C3E-4FC9-AD9F-C09EC18B1399}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{0F37505F-B9AC-440A-9A53-0A1039AF79B0}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{B128C7AB-569C-4147-8A87-E56A796A8D1E}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="1" activeTab="3" xr2:uid="{B128C7AB-569C-4147-8A87-E56A796A8D1E}"/>
   </bookViews>
   <sheets>
     <sheet name="Content-Mucosa Comparison" sheetId="1" r:id="rId1"/>
     <sheet name="Content-Mucosa Separately" sheetId="2" r:id="rId2"/>
+    <sheet name="Lab Squirrels Only" sheetId="4" r:id="rId3"/>
+    <sheet name="Lab Content-Mucosa Separately" sheetId="3" r:id="rId4"/>
+    <sheet name="Overall" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -35,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="149" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="269" uniqueCount="33">
   <si>
     <t>Group</t>
   </si>
@@ -82,9 +85,6 @@
     <t>Mucosa</t>
   </si>
   <si>
-    <t>Season</t>
-  </si>
-  <si>
     <t>All</t>
   </si>
   <si>
@@ -122,6 +122,21 @@
   </si>
   <si>
     <t>Summer_Lab vs. IBA</t>
+  </si>
+  <si>
+    <t>Lab</t>
+  </si>
+  <si>
+    <t>Summer vs. IBA</t>
+  </si>
+  <si>
+    <t>Summer vs. Torpor</t>
+  </si>
+  <si>
+    <t>Bray-Curtis Dispersion</t>
+  </si>
+  <si>
+    <t>Bray-Curtis ANOSIM</t>
   </si>
 </sst>
 </file>
@@ -145,7 +160,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -164,8 +179,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.14999847407452621"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="3">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -191,11 +212,22 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -212,6 +244,13 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -529,7 +568,7 @@
   <dimension ref="A1:I11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H19" sqref="H19"/>
+      <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -617,7 +656,7 @@
         <v>12</v>
       </c>
       <c r="I3">
-        <v>0.97299999999999998</v>
+        <v>0.97919999999999996</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.3">
@@ -643,7 +682,7 @@
         <v>12</v>
       </c>
       <c r="I4">
-        <v>0.94099999999999995</v>
+        <v>0.94420000000000004</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.3">
@@ -669,7 +708,7 @@
         <v>12</v>
       </c>
       <c r="I5">
-        <v>0.95099999999999996</v>
+        <v>0.95979999999999999</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.3">
@@ -695,7 +734,7 @@
         <v>12</v>
       </c>
       <c r="I6" s="4">
-        <v>0.9</v>
+        <v>1</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.3">
@@ -778,8 +817,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5A86CB5D-939B-4B14-AC59-EE530224E751}">
   <dimension ref="A1:K31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D24" sqref="D24"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J3" sqref="J3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -797,7 +836,7 @@
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="5" t="s">
         <v>1</v>
       </c>
       <c r="C1" s="2" t="s">
@@ -824,7 +863,7 @@
         <v>13</v>
       </c>
       <c r="B2" s="9" t="s">
-        <v>15</v>
+        <v>0</v>
       </c>
       <c r="C2" s="9" t="s">
         <v>10</v>
@@ -836,13 +875,13 @@
         <v>13</v>
       </c>
       <c r="H2" t="s">
-        <v>15</v>
+        <v>0</v>
       </c>
       <c r="I2" t="s">
         <v>12</v>
       </c>
       <c r="J2">
-        <v>1E-3</v>
+        <v>1E-4</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.3">
@@ -850,7 +889,7 @@
         <v>14</v>
       </c>
       <c r="B3" s="10" t="s">
-        <v>15</v>
+        <v>0</v>
       </c>
       <c r="C3" s="10" t="s">
         <v>10</v>
@@ -862,47 +901,35 @@
         <v>14</v>
       </c>
       <c r="H3" t="s">
-        <v>15</v>
+        <v>0</v>
       </c>
       <c r="I3" t="s">
         <v>12</v>
       </c>
       <c r="J3">
-        <v>1E-3</v>
+        <v>1E-4</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A4" s="8" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B4" s="8" t="s">
-        <v>15</v>
+        <v>0</v>
       </c>
       <c r="C4" s="8" t="s">
         <v>10</v>
       </c>
       <c r="D4" s="8">
         <v>1.2619999999999999E-2</v>
-      </c>
-      <c r="G4" t="s">
-        <v>16</v>
-      </c>
-      <c r="H4" t="s">
-        <v>15</v>
-      </c>
-      <c r="I4" t="s">
-        <v>12</v>
-      </c>
-      <c r="J4">
-        <v>1E-3</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A5" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="B5" s="9" t="s">
-        <v>15</v>
+      <c r="B5" s="10" t="s">
+        <v>0</v>
       </c>
       <c r="C5" s="9" t="s">
         <v>11</v>
@@ -916,7 +943,7 @@
         <v>14</v>
       </c>
       <c r="B6" s="10" t="s">
-        <v>15</v>
+        <v>0</v>
       </c>
       <c r="C6" s="10" t="s">
         <v>11</v>
@@ -927,10 +954,10 @@
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A7" s="8" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B7" s="8" t="s">
-        <v>15</v>
+        <v>0</v>
       </c>
       <c r="C7" s="8" t="s">
         <v>11</v>
@@ -939,7 +966,7 @@
         <v>9.0299999999999998E-3</v>
       </c>
       <c r="G7" s="5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="H7" s="5"/>
       <c r="I7" s="5"/>
@@ -947,7 +974,7 @@
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A8" s="7"/>
-      <c r="B8" s="7"/>
+      <c r="B8" s="16"/>
       <c r="C8" s="7"/>
       <c r="D8" s="7"/>
       <c r="G8" s="2" t="s">
@@ -960,26 +987,26 @@
         <v>9</v>
       </c>
       <c r="J8" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.3">
       <c r="G9" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="H9" s="6" t="s">
-        <v>15</v>
+      <c r="H9" t="s">
+        <v>0</v>
       </c>
       <c r="I9" s="6" t="s">
         <v>12</v>
       </c>
       <c r="J9" s="11" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A10" s="5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B10" s="5"/>
       <c r="C10" s="5"/>
@@ -988,27 +1015,27 @@
       <c r="H10" s="4"/>
       <c r="I10" s="4"/>
       <c r="J10" s="13" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B11" s="2" t="s">
+      <c r="B11" s="5" t="s">
         <v>1</v>
       </c>
       <c r="C11" s="2" t="s">
         <v>9</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="G11" s="4"/>
       <c r="H11" s="4"/>
       <c r="I11" s="4"/>
       <c r="J11" s="13" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.3">
@@ -1016,39 +1043,39 @@
         <v>13</v>
       </c>
       <c r="B12" s="6" t="s">
-        <v>15</v>
+        <v>0</v>
       </c>
       <c r="C12" s="6" t="s">
         <v>10</v>
       </c>
       <c r="D12" s="6" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="G12" s="4"/>
       <c r="H12" s="4"/>
       <c r="I12" s="4"/>
       <c r="J12" s="10" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A13" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="B13" s="3" t="s">
         <v>15</v>
+      </c>
+      <c r="B13" s="4" t="s">
+        <v>0</v>
       </c>
       <c r="C13" s="3" t="s">
         <v>10</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="G13" s="4"/>
       <c r="H13" s="4"/>
       <c r="I13" s="4"/>
       <c r="J13" s="13" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.3">
@@ -1056,19 +1083,19 @@
         <v>13</v>
       </c>
       <c r="B14" s="6" t="s">
-        <v>15</v>
+        <v>0</v>
       </c>
       <c r="C14" s="6" t="s">
         <v>11</v>
       </c>
       <c r="D14" s="6" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="G14" s="4"/>
       <c r="H14" s="4"/>
       <c r="I14" s="4"/>
       <c r="J14" s="13" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.3">
@@ -1076,13 +1103,13 @@
       <c r="B15" s="4"/>
       <c r="C15" s="4"/>
       <c r="D15" s="4" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="G15" s="4"/>
       <c r="H15" s="4"/>
       <c r="I15" s="4"/>
       <c r="J15" s="13" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.3">
@@ -1090,13 +1117,13 @@
       <c r="B16" s="4"/>
       <c r="C16" s="4"/>
       <c r="D16" s="4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="G16" s="3"/>
       <c r="H16" s="3"/>
       <c r="I16" s="3"/>
       <c r="J16" s="15" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.3">
@@ -1104,109 +1131,145 @@
       <c r="B17" s="4"/>
       <c r="C17" s="4"/>
       <c r="D17" s="4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="G17" t="s">
         <v>14</v>
       </c>
       <c r="H17" t="s">
-        <v>15</v>
+        <v>0</v>
       </c>
       <c r="I17" t="s">
         <v>12</v>
       </c>
       <c r="J17" s="12" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A18" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>15</v>
+        <v>0</v>
       </c>
       <c r="C18" s="3" t="s">
         <v>11</v>
       </c>
       <c r="D18" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E18" s="1"/>
       <c r="J18" s="12" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.3">
       <c r="J19" s="12" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.3">
       <c r="J20" s="12" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A21" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C21" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D21" s="2" t="s">
+        <v>2</v>
+      </c>
       <c r="J21" s="12" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A22" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="B22" t="s">
+        <v>0</v>
+      </c>
+      <c r="C22" t="s">
+        <v>10</v>
+      </c>
+      <c r="D22">
+        <v>0.12089999999999999</v>
+      </c>
       <c r="J22" s="12" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A23" t="s">
+        <v>28</v>
+      </c>
+      <c r="B23" t="s">
+        <v>0</v>
+      </c>
+      <c r="C23" t="s">
+        <v>11</v>
+      </c>
+      <c r="D23">
+        <v>9.3200000000000005E-2</v>
+      </c>
       <c r="G23" s="3"/>
       <c r="H23" s="3"/>
       <c r="I23" s="3"/>
       <c r="J23" s="15" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.3">
       <c r="G24" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="H24" t="s">
-        <v>15</v>
+        <v>0</v>
       </c>
       <c r="I24" t="s">
         <v>12</v>
       </c>
       <c r="J24" s="12" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.3">
       <c r="J25" s="12" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.3">
       <c r="J26" s="12" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.3">
       <c r="J27" s="14" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.3">
       <c r="J28" s="12" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.3">
       <c r="J29" s="12" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="30" spans="1:11" x14ac:dyDescent="0.3">
       <c r="J30" s="12" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="31" spans="1:11" x14ac:dyDescent="0.3">
@@ -1214,9 +1277,521 @@
       <c r="H31" s="3"/>
       <c r="I31" s="3"/>
       <c r="J31" s="15" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="K31" s="3"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{75B1EBFB-AFAE-4AEA-A796-2B1C0C8A3CB5}">
+  <dimension ref="A1:I9"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:I1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="8" max="8" width="22.109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>28</v>
+      </c>
+      <c r="B2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D2">
+        <v>0.12089999999999999</v>
+      </c>
+      <c r="F2" t="s">
+        <v>28</v>
+      </c>
+      <c r="G2" t="s">
+        <v>0</v>
+      </c>
+      <c r="H2" t="s">
+        <v>12</v>
+      </c>
+      <c r="I2">
+        <v>1E-3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>28</v>
+      </c>
+      <c r="B3" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D3">
+        <v>9.3200000000000005E-2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="F4" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="G4" s="5"/>
+      <c r="H4" s="5"/>
+      <c r="I4" s="5"/>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="F5" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="G5" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="H5" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="I5" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="F6" s="17" t="s">
+        <v>28</v>
+      </c>
+      <c r="G6" s="17" t="s">
+        <v>0</v>
+      </c>
+      <c r="H6" s="18" t="s">
+        <v>12</v>
+      </c>
+      <c r="I6" s="18" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="I7" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="I8" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="I9" t="s">
+        <v>24</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CD663AA7-7EAD-44D7-AF83-AB38F355B175}">
+  <dimension ref="A1:J13"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H11" sqref="H11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="4" max="4" width="16.5546875" customWidth="1"/>
+    <col min="9" max="9" width="23.88671875" customWidth="1"/>
+    <col min="10" max="10" width="17.33203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A2" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="B2" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="D2" s="6">
+        <v>0.20799999999999999</v>
+      </c>
+      <c r="G2" s="19" t="s">
+        <v>13</v>
+      </c>
+      <c r="H2" s="19" t="s">
+        <v>0</v>
+      </c>
+      <c r="I2" s="19" t="s">
+        <v>12</v>
+      </c>
+      <c r="J2" s="19">
+        <v>1E-3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A3" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D3" s="3">
+        <v>0.18490000000000001</v>
+      </c>
+      <c r="G3" s="19" t="s">
+        <v>14</v>
+      </c>
+      <c r="H3" s="19" t="s">
+        <v>0</v>
+      </c>
+      <c r="I3" s="19" t="s">
+        <v>12</v>
+      </c>
+      <c r="J3" s="19">
+        <v>1.6999999999999999E-3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A4" s="14" t="s">
+        <v>13</v>
+      </c>
+      <c r="B4" s="14" t="s">
+        <v>0</v>
+      </c>
+      <c r="C4" s="14" t="s">
+        <v>11</v>
+      </c>
+      <c r="D4" s="14">
+        <v>3.1399999999999997E-2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A5" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D5" s="3">
+        <v>0.74399999999999999</v>
+      </c>
+      <c r="G5" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="H5" s="5"/>
+      <c r="I5" s="5"/>
+      <c r="J5" s="5"/>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="G6" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="H6" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="I6" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="J6" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="G7" t="s">
+        <v>13</v>
+      </c>
+      <c r="H7" t="s">
+        <v>0</v>
+      </c>
+      <c r="I7" t="s">
+        <v>12</v>
+      </c>
+      <c r="J7" s="21" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A8" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="B8" s="5"/>
+      <c r="C8" s="5"/>
+      <c r="D8" s="5"/>
+      <c r="J8" s="21" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A9" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="J9" s="14" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A10" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="B10" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="C10" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="D10" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="G10" s="3"/>
+      <c r="H10" s="3"/>
+      <c r="I10" s="3"/>
+      <c r="J10" s="8" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A11" s="20"/>
+      <c r="B11" s="20"/>
+      <c r="C11" s="20"/>
+      <c r="D11" s="20" t="s">
+        <v>23</v>
+      </c>
+      <c r="G11" t="s">
+        <v>14</v>
+      </c>
+      <c r="H11" t="s">
+        <v>0</v>
+      </c>
+      <c r="I11" t="s">
+        <v>12</v>
+      </c>
+      <c r="J11" s="22" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="J12" s="22" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="J13" s="16"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9F01B6E3-D394-4658-AD8E-416900378F21}">
+  <dimension ref="A1:I9"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H3" sqref="H3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="8" max="8" width="22" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D2">
+        <v>1.2619999999999999E-2</v>
+      </c>
+      <c r="F2" t="s">
+        <v>15</v>
+      </c>
+      <c r="G2" t="s">
+        <v>0</v>
+      </c>
+      <c r="H2" t="s">
+        <v>32</v>
+      </c>
+      <c r="I2">
+        <v>1E-3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B3" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D3">
+        <v>9.0299999999999998E-3</v>
+      </c>
+      <c r="H3" t="s">
+        <v>31</v>
+      </c>
+      <c r="I3">
+        <v>6.0000000000000001E-3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A6" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="B6" s="5"/>
+      <c r="C6" s="5"/>
+      <c r="D6" s="5"/>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A7" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>15</v>
+      </c>
+      <c r="B8" t="s">
+        <v>0</v>
+      </c>
+      <c r="C8" t="s">
+        <v>10</v>
+      </c>
+      <c r="D8" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>15</v>
+      </c>
+      <c r="B9" t="s">
+        <v>0</v>
+      </c>
+      <c r="C9" t="s">
+        <v>11</v>
+      </c>
+      <c r="D9" t="s">
+        <v>21</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>